<commit_message>
Updated 3D printing progress and costs
</commit_message>
<xml_diff>
--- a/Project Costs/Prototype cost.xlsx
+++ b/Project Costs/Prototype cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git Repos\Infinity-Northstar\Project Costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F8DE8B-10F9-416A-9FD1-F18415EE8A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B5C629-3EDF-4733-9110-3229E9276E18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{028F46EA-D03F-4DCA-92EC-6E8536515A69}"/>
+    <workbookView xWindow="5460" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{028F46EA-D03F-4DCA-92EC-6E8536515A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Sr.no</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Transcend 128GB M.2 SSD Type 2260</t>
   </si>
   <si>
-    <t>PCB Antenna</t>
-  </si>
-  <si>
     <t>Intel 3165AC Dual Band Wireless M.2</t>
   </si>
   <si>
@@ -90,13 +87,64 @@
   </si>
   <si>
     <t>3D printed parts from Wnex</t>
+  </si>
+  <si>
+    <t>3D printed parts from Wnex 2</t>
+  </si>
+  <si>
+    <t>140.09 (+17.55 Import Taxes)</t>
+  </si>
+  <si>
+    <t>Prototype Cost</t>
+  </si>
+  <si>
+    <t>Northstar Kit B</t>
+  </si>
+  <si>
+    <t>UDOO Kit WiFi M.2 BT + Antenna</t>
+  </si>
+  <si>
+    <t>Manufacturing Cost (per unit) - Excludes Import Taxes</t>
+  </si>
+  <si>
+    <t>Estimated Shipping Price</t>
+  </si>
+  <si>
+    <t>Price including shipping (USD)</t>
+  </si>
+  <si>
+    <t>Comparison with other AR Head Sets</t>
+  </si>
+  <si>
+    <t>Sr. no</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Microsoft Holo Lens 2</t>
+  </si>
+  <si>
+    <t>Magic Leap 1</t>
+  </si>
+  <si>
+    <t>Carrying case</t>
+  </si>
+  <si>
+    <t>FOV  Diagonal(Degrees)</t>
+  </si>
+  <si>
+    <t>NorthStar</t>
+  </si>
+  <si>
+    <t>Split Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,13 +160,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -142,6 +204,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED45DDB-BF86-4495-B250-33C9278540B3}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,215 +544,492 @@
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <f>213.44+56.71</f>
-        <v>270.14999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3">
-        <f>366.06+58.15</f>
-        <v>424.21</v>
+        <f>(213.44+56.71) *D3</f>
+        <v>270.14999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
-        <v>15.79</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
       </c>
       <c r="E4" s="3">
-        <f>C4</f>
-        <v>15.79</v>
+        <f>(366.06+58.15)*D4</f>
+        <v>424.21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>31.59</v>
+        <v>15.79</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
       <c r="E5" s="3">
-        <f>C5</f>
-        <v>31.59</v>
+        <f>C5*D5</f>
+        <v>15.79</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>31.59</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" s="3">
-        <f>445.29+89.05</f>
-        <v>534.34</v>
+        <f>C6*D6</f>
+        <v>31.59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3">
-        <v>118.24</v>
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
       </c>
       <c r="E7" s="3">
-        <f>C7</f>
-        <v>118.24</v>
+        <f>(445.29+89.05)*D7</f>
+        <v>534.34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
-        <v>7.7</v>
+        <v>118.24</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="E8" s="3">
-        <f>C8</f>
-        <v>7.7</v>
+        <f>C8*D8</f>
+        <v>118.24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
-        <v>26.13</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="E9" s="3">
-        <f>C9</f>
-        <v>26.13</v>
+        <f>C9*D9</f>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3">
-        <v>62.33</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
-        <f>C10</f>
-        <v>62.33</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4">
+        <v>26.13</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <f>C10*D10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3">
+        <v>137.5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <f>C11*D11</f>
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <f>(140.09+17.55)*D12</f>
+        <v>157.64000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3">
-        <v>140.09</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3">
-        <f>C11</f>
-        <v>140.09</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C13" s="3">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <f>C13*D13</f>
+        <v>33.950000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E12">
-        <f>E2+E3+E4+E5+E6+E7+E8+E9+E10+E11</f>
-        <v>1630.57</v>
+      <c r="E14">
+        <f>E3+E4+E5+E6+E7+E8+E9+E10+E22+E12+E13+E11</f>
+        <v>1797.8100000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="7">
+        <v>677</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7">
+        <f>C19*D19</f>
+        <v>677</v>
+      </c>
+      <c r="F19" s="7">
+        <v>100.16</v>
+      </c>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>2</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="7">
+        <v>15.79</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <f>C20*D20</f>
+        <v>15.79</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <f>E19+F19+E20</f>
+        <v>792.94999999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="3">
+        <v>418</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <f>C21*D21</f>
+        <v>418</v>
+      </c>
+      <c r="F21" s="3">
+        <v>128.11000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="3">
+        <v>57.5</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <f>C22*D22</f>
+        <v>57.5</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>5</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="3">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <f>C23*D23</f>
+        <v>78.900000000000006</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>E21+F21+E23+E22</f>
+        <v>682.51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24">
+        <f>E19+E20+E21+E22+E23</f>
+        <v>1247.19</v>
+      </c>
+      <c r="F24">
+        <f>F19+F20+F21+F22+F23+E24</f>
+        <v>1475.46</v>
+      </c>
+      <c r="G24">
+        <f>G20+G23</f>
+        <v>1475.46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29">
+        <v>3500</v>
+      </c>
+      <c r="D29">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30">
+        <v>2495</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>1500</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A27:F27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>